<commit_message>
Added missing score in results
</commit_message>
<xml_diff>
--- a/KWG/Complex/Axiomatization/Results/Axioms.txt_cq_GPT4o_results.xlsx
+++ b/KWG/Complex/Axiomatization/Results/Axioms.txt_cq_GPT4o_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elhamghiasi/Documents/GitHub/graph-rag-iswc-2025/util-scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anmolsaini/git/graph-rag-iswc-2025/KWG/Complex/Axiomatization/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1C83F4-D87A-534D-9CE8-11D72CC46FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053FC2AE-FE62-1444-9B14-F83660F04809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1040" windowWidth="34200" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3975,6 +3975,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -4335,8 +4336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4678,6 +4679,9 @@
       <c r="D17" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="E17">
+        <v>-1</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">

</xml_diff>